<commit_message>
Note 2 ngay cuoi tuan 9-10 Sept 2023
</commit_message>
<xml_diff>
--- a/to-dolist.xlsx
+++ b/to-dolist.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tiennv65\workingspace\secbramet\secbramet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\workingspace\secondbrainmethod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9E234E-CA69-41E8-A4E5-A3AD313E5A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="thang9" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>time</t>
   </si>
@@ -58,16 +57,55 @@
   </si>
   <si>
     <t>booking</t>
+  </si>
+  <si>
+    <t>Tóm tắt uốn sách lối sống tối giản của Steve Job</t>
+  </si>
+  <si>
+    <t>Bai hát chari chari lady</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The 5 magical apps that changed my life
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Video youtube</t>
+    </r>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>7 level of reading book.
+How to remember every thing what you read</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,10 +131,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,22 +417,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" customWidth="1"/>
-    <col min="4" max="4" width="32.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="43" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -408,7 +450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -421,8 +463,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -433,7 +478,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -447,7 +492,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -457,8 +502,57 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45179</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45179</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>45179</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>